<commit_message>
finished chapter 1 to chapter 3 and added cover and index
</commit_message>
<xml_diff>
--- a/report/table_supply_sources.xlsx
+++ b/report/table_supply_sources.xlsx
@@ -60,13 +60,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -115,15 +121,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,12 +426,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -433,8 +439,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
@@ -442,8 +448,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -451,8 +457,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
@@ -460,8 +466,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
@@ -469,8 +475,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -479,8 +485,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>